<commit_message>
Update Dic 13 2021
</commit_message>
<xml_diff>
--- a/ENG corta/data/working-experience.xlsx
+++ b/ENG corta/data/working-experience.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F15CEDB-6649-4705-A701-B144BD9A33E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD80CBC0-2481-404F-A78F-2DF66725DD5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25290" yWindow="3510" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>what</t>
   </si>
@@ -35,18 +35,6 @@
   </si>
   <si>
     <t>why</t>
-  </si>
-  <si>
-    <t>Teaching Assistant</t>
-  </si>
-  <si>
-    <t>2011 - 2014</t>
-  </si>
-  <si>
-    <t>University of Stirling</t>
-  </si>
-  <si>
-    <t>Stirling, UK</t>
   </si>
   <si>
     <t>Cathedratic Professor</t>
@@ -389,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,46 +411,32 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>